<commit_message>
major update to style catalogue and associated tests
</commit_message>
<xml_diff>
--- a/inst/extdata/tester_styles.xlsx
+++ b/inst/extdata/tester_styles.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="-3560" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>text_colour1</t>
   </si>
@@ -43,13 +43,28 @@
   </si>
   <si>
     <t>bg2</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>bolditalic</t>
+  </si>
+  <si>
+    <t>rowheight_30</t>
+  </si>
+  <si>
+    <t>rowheight_40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +122,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF8168CB"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -140,17 +163,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -161,6 +173,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -191,16 +214,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -558,77 +584,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B16"/>
+  <dimension ref="A2:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" ht="15" customHeight="1" thickBot="1">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18">
-      <c r="A14" s="5" t="s">
+    </row>
+    <row r="14" spans="1:1" ht="18">
+      <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="16">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" spans="1:1" ht="16">
+      <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16">
-        <v>15</v>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="30" customHeight="1">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="40" customHeight="1">
+      <c r="A26" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>